<commit_message>
adding lsatest.R to show how to get multiple iterations of the lsa algorithm
</commit_message>
<xml_diff>
--- a/alphas.xlsx
+++ b/alphas.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feignedpoet\Documents\lda-lsa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cody/Documents/lda-lsa/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6990" windowHeight="11130"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21860" windowHeight="16660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -169,13 +172,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>1.0000000000000001E-5</c:v>
+                  <c:v>1.0E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1E-4</c:v>
+                  <c:v>0.0001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1E-3</c:v>
+                  <c:v>0.001</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.01</c:v>
@@ -187,7 +190,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.5</c:v>
@@ -202,7 +205,7 @@
                   <c:v>4.38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>6.25</c:v>
@@ -211,16 +214,16 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>40.630000000000003</c:v>
+                  <c:v>40.63</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>43.75</c:v>
@@ -229,19 +232,19 @@
                   <c:v>46.88</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>51</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>56.25</c:v>
@@ -250,10 +253,10 @@
                   <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>75</c:v>
+                  <c:v>75.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -268,7 +271,7 @@
                   <c:v>0.226936</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28992220000000002</c:v>
+                  <c:v>0.2899222</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.226936</c:v>
@@ -277,25 +280,25 @@
                   <c:v>0.226936</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.22702720000000001</c:v>
+                  <c:v>0.2270272</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.2931899</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.31527080000000002</c:v>
+                  <c:v>0.3152708</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.40862169999999998</c:v>
+                  <c:v>0.4086217</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39812690000000001</c:v>
+                  <c:v>0.3981269</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.3719151</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.35381170000000001</c:v>
+                  <c:v>0.3538117</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.4112131</c:v>
@@ -310,10 +313,10 @@
                   <c:v>0.3480859</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.38067820000000002</c:v>
+                  <c:v>0.3806782</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.39265149999999999</c:v>
+                  <c:v>0.3926515</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.4343766</c:v>
@@ -328,13 +331,13 @@
                   <c:v>0.4343766</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.45626030000000001</c:v>
+                  <c:v>0.4562603</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.45626030000000001</c:v>
+                  <c:v>0.4562603</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.45626030000000001</c:v>
+                  <c:v>0.4562603</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0.4343766</c:v>
@@ -364,11 +367,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116836336"/>
-        <c:axId val="116832024"/>
+        <c:axId val="-2060373808"/>
+        <c:axId val="-2061722304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116836336"/>
+        <c:axId val="-2060373808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,12 +428,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116832024"/>
+        <c:crossAx val="-2061722304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116832024"/>
+        <c:axId val="-2061722304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +490,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116836336"/>
+        <c:crossAx val="-2060373808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1096,14 +1099,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>147637</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>541337</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>452437</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>173037</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
@@ -1173,9 +1176,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1208,9 +1211,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1392,18 +1395,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>0.3480859</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1.0000000000000001E-5</v>
       </c>
@@ -1419,7 +1422,7 @@
         <v>0.226936</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1E-4</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>0.28992220000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1E-3</v>
       </c>
@@ -1435,7 +1438,7 @@
         <v>0.226936</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.01</v>
       </c>
@@ -1443,7 +1446,7 @@
         <v>0.226936</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.1</v>
       </c>
@@ -1451,7 +1454,7 @@
         <v>0.22702720000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.5</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>0.2931899</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1467,7 +1470,7 @@
         <v>0.31527080000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2.5</v>
       </c>
@@ -1475,7 +1478,7 @@
         <v>0.40862169999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3.13</v>
       </c>
@@ -1483,7 +1486,7 @@
         <v>0.39812690000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3.75</v>
       </c>
@@ -1491,7 +1494,7 @@
         <v>0.3719151</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4.38</v>
       </c>
@@ -1499,7 +1502,7 @@
         <v>0.35381170000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>0.4112131</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6.25</v>
       </c>
@@ -1515,7 +1518,7 @@
         <v>0.3002127</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7.5</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>0.3040062</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1531,7 +1534,7 @@
         <v>0.3480859</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>25</v>
       </c>
@@ -1539,7 +1542,7 @@
         <v>0.38067820000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>37.5</v>
       </c>
@@ -1547,7 +1550,7 @@
         <v>0.39265149999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>40.630000000000003</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>0.4343766</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>43.75</v>
       </c>
@@ -1563,7 +1566,7 @@
         <v>0.4343766</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>46.88</v>
       </c>
@@ -1571,7 +1574,7 @@
         <v>0.4343766</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>49</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>0.4343766</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>49.5</v>
       </c>
@@ -1587,7 +1590,7 @@
         <v>0.45626030000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>50</v>
       </c>
@@ -1595,7 +1598,7 @@
         <v>0.45626030000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>50.5</v>
       </c>
@@ -1603,7 +1606,7 @@
         <v>0.45626030000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>51</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>0.4343766</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>56.25</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>0.112801</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>62.5</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>0.112801</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>75</v>
       </c>
@@ -1635,7 +1638,7 @@
         <v>0.108663</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>100</v>
       </c>
@@ -1643,7 +1646,7 @@
         <v>0.1138591</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>500</v>
       </c>

</xml_diff>